<commit_message>
Eliteserien data got a new place i dir.
</commit_message>
<xml_diff>
--- a/stored_data/eliteserien/2022/fixture_data/Eliteserien_fixtures.xlsx
+++ b/stored_data/eliteserien/2022/fixture_data/Eliteserien_fixtures.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="75">
   <si>
     <t xml:space="preserve"> @D_Thon</t>
   </si>
@@ -1217,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z982"/>
+  <dimension ref="A1:AA982"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1239,7 +1239,7 @@
     <col min="19" max="19" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1266,7 +1266,7 @@
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="12">
         <v>1</v>
@@ -1343,8 +1343,11 @@
       <c r="Z2" s="103">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA2" s="103">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>50</v>
       </c>
@@ -1419,8 +1422,11 @@
       <c r="Z3" s="96" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA3" s="96" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
         <v>51</v>
       </c>
@@ -1499,8 +1505,11 @@
       <c r="Z4" s="92" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA4" s="92" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
         <v>52</v>
       </c>
@@ -1579,8 +1588,11 @@
       <c r="Z5" s="97" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA5" s="97" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="30" t="s">
         <v>53</v>
       </c>
@@ -1657,8 +1669,11 @@
       <c r="Z6" s="95" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA6" s="95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
         <v>54</v>
       </c>
@@ -1737,8 +1752,11 @@
       <c r="Z7" s="95" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA7" s="95" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
         <v>55</v>
       </c>
@@ -1817,8 +1835,11 @@
       <c r="Z8" s="96" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA8" s="96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
         <v>56</v>
       </c>
@@ -1893,8 +1914,11 @@
       <c r="Z9" s="96" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA9" s="96" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="34" t="s">
         <v>57</v>
       </c>
@@ -1971,8 +1995,11 @@
       <c r="Z10" s="92" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA10" s="92" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>58</v>
       </c>
@@ -2049,8 +2076,11 @@
       <c r="Z11" s="93" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA11" s="93" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="39" t="s">
         <v>59</v>
       </c>
@@ -2129,8 +2159,11 @@
       <c r="Z12" s="93" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA12" s="93" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="41" t="s">
         <v>60</v>
       </c>
@@ -2209,8 +2242,11 @@
       <c r="Z13" s="97" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA13" s="97" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="44" t="s">
         <v>61</v>
       </c>
@@ -2289,8 +2325,11 @@
       <c r="Z14" s="93" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA14" s="93" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
         <v>62</v>
       </c>
@@ -2367,8 +2406,11 @@
       <c r="Z15" s="96" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA15" s="96" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="48" t="s">
         <v>63</v>
       </c>
@@ -2445,8 +2487,11 @@
       <c r="Z16" s="96" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA16" s="96" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="49" t="s">
         <v>64</v>
       </c>
@@ -2521,8 +2566,11 @@
       <c r="Z17" s="96" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA17" s="96" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="53" t="s">
         <v>65</v>
       </c>
@@ -2597,8 +2645,11 @@
       <c r="Z18" s="95" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AA18" s="95" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -2618,7 +2669,7 @@
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
     </row>
-    <row r="20" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
@@ -2634,7 +2685,7 @@
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -2650,7 +2701,7 @@
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -2666,7 +2717,7 @@
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -2682,7 +2733,7 @@
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
     </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -2698,7 +2749,7 @@
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -2714,7 +2765,7 @@
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -2730,7 +2781,7 @@
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -2746,7 +2797,7 @@
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
@@ -2762,7 +2813,7 @@
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -2778,7 +2829,7 @@
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
     </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -2794,7 +2845,7 @@
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -2810,7 +2861,7 @@
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>

</xml_diff>